<commit_message>
fix bug and add new blog
</commit_message>
<xml_diff>
--- a/WebAppCore/wwwroot/export-files/Bill_3.xlsx
+++ b/WebAppCore/wwwroot/export-files/Bill_3.xlsx
@@ -5,28 +5,28 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngoct\Documents\Visual Studio 2017\Projects\TeduCore\TeduCore.WebApp\wwwroot\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev_Web_AppliCation-Core\WebAppCore\wwwroot\export-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="TEDUOrder" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511" iterateDelta="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Sales Order</t>
   </si>
   <si>
-    <t xml:space="preserve">Address: Xuan La Tay Ho Ha Noi
+    <t>Address: Xuan La Tay Ho Ha Noi
 ĐT: 0966 036 626</t>
   </si>
   <si>
@@ -98,7 +98,7 @@
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -219,99 +219,96 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="4" applyBorder="1" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="4" applyBorder="1" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="4" applyBorder="1" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+  <cellXfs count="30">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -329,55 +326,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>809625</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1619250</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>828675</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1181100" y="19050"/>
-          <a:ext cx="809626" cy="809626"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -646,319 +594,324 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E4"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" customWidth="1" style="2"/>
-    <col min="2" max="2" width="42.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1" style="3"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1" style="3"/>
-    <col min="5" max="5" width="19.140625" customWidth="1" style="3"/>
+    <col min="1" max="1" width="5.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="67.5" customHeight="1">
-      <c r="A1" s="25"/>
-      <c r="B1" s="25"/>
-      <c r="C1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="27" t="s">
+    <row r="1" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="30" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="30"/>
-    </row>
-    <row r="4" ht="20.1" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="B3" s="24"/>
+    </row>
+    <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-    </row>
-    <row r="5" ht="20.1" customHeight="1">
-      <c r="A5" s="20" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-    </row>
-    <row r="6" ht="20.1" customHeight="1">
-      <c r="A6" s="16" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+    </row>
+    <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-    </row>
-    <row r="8" ht="18" customHeight="1" s="2" customFormat="1">
-      <c r="A8" s="5" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" ht="18" customHeight="1">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" ht="18" customHeight="1">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" ht="18" customHeight="1">
-      <c r="A11" s="8">
+    <row r="11" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>3</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6">
-        <f ref="E11:E23" t="shared" si="0">C11*D11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" ht="18" customHeight="1">
-      <c r="A12" s="8">
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5">
+        <f t="shared" ref="E11:E23" si="0">C11*D11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>4</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" ht="18" customHeight="1">
-      <c r="A13" s="8">
+      <c r="B12" s="6"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
         <v>5</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" ht="18" customHeight="1">
-      <c r="A14" s="8">
+      <c r="B13" s="6"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
         <v>6</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" ht="18" customHeight="1">
-      <c r="A15" s="8">
+      <c r="B14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
         <v>7</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" ht="18" customHeight="1">
-      <c r="A16" s="8">
+      <c r="B15" s="6"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
         <v>8</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" ht="18" customHeight="1">
-      <c r="A17" s="8">
+      <c r="B16" s="6"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
         <v>9</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" ht="18" customHeight="1">
-      <c r="A18" s="8">
+      <c r="B17" s="6"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
         <v>10</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" ht="18" customHeight="1">
-      <c r="A19" s="8">
+      <c r="B18" s="6"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
         <v>11</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" ht="18" customHeight="1">
-      <c r="A20" s="8">
+      <c r="B19" s="6"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
         <v>12</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" ht="18" customHeight="1">
-      <c r="A21" s="8">
+      <c r="B20" s="6"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
         <v>13</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" ht="18" customHeight="1">
-      <c r="A22" s="8">
+      <c r="B21" s="6"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
         <v>14</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" ht="18" customHeight="1">
-      <c r="A23" s="9">
+      <c r="B22" s="6"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
         <v>15</v>
       </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" ht="18" customHeight="1">
-      <c r="A24" s="18" t="s">
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="4">
+      <c r="B24" s="25"/>
+      <c r="C24" s="3">
         <f>SUM(C9:C23)</f>
         <v>0</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4" t="s">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" ht="30.75" customHeight="1">
-      <c r="A26" s="19" t="s">
+    <row r="26" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-    </row>
-    <row r="28">
-      <c r="C28" s="22" t="s">
+      <c r="B26" s="17"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="23" t="s">
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="24" t="s">
+      <c r="B29" s="28"/>
+      <c r="C29" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
     </row>
   </sheetData>
-  <mergeCells>
+  <mergeCells count="12">
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:E29"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:E1"/>
@@ -966,25 +919,20 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:E29"/>
   </mergeCells>
   <pageMargins left="0.55069444444444449" right="0.2361111111111111" top="0.47222222222222221" bottom="0.35416666666666669" header="0.31458333333333333" footer="0.27500000000000002"/>
   <pageSetup paperSize="9" firstPageNumber="4294963191" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="4294963191" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -994,10 +942,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="4294963191" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>